<commit_message>
Já add novas regras para gerar a escala corretamente
</commit_message>
<xml_diff>
--- a/ESCALA_TORRE_V5.xlsx
+++ b/ESCALA_TORRE_V5.xlsx
@@ -20,7 +20,7 @@
     <t>ESCALA DE TRABALHO - TORRE DE CONTROLE</t>
   </si>
   <si>
-    <t>MÊS: NOVEMBRO/2025</t>
+    <t>MÊS: DEZEMBRO/2025</t>
   </si>
   <si>
     <t>DATA</t>
@@ -125,43 +125,43 @@
     <t>BRANCÃO</t>
   </si>
   <si>
+    <t>EDUARDO</t>
+  </si>
+  <si>
+    <t>ALLAN</t>
+  </si>
+  <si>
     <t>MARCO</t>
   </si>
   <si>
-    <t>ALLAN</t>
-  </si>
-  <si>
-    <t>EDUARDO</t>
+    <t>00H_OP2</t>
+  </si>
+  <si>
+    <t>THAIS</t>
+  </si>
+  <si>
+    <t>RICHER</t>
+  </si>
+  <si>
+    <t>B.HORNES</t>
+  </si>
+  <si>
+    <t>GUILHERME</t>
+  </si>
+  <si>
+    <t>FELIPE</t>
+  </si>
+  <si>
+    <t>B.SELAYARAN</t>
+  </si>
+  <si>
+    <t>06H_OP1</t>
+  </si>
+  <si>
+    <t>CLEITON</t>
   </si>
   <si>
     <t>TONINHO</t>
-  </si>
-  <si>
-    <t>CLEITON</t>
-  </si>
-  <si>
-    <t>00H_OP2</t>
-  </si>
-  <si>
-    <t>THAIS</t>
-  </si>
-  <si>
-    <t>FELIPE</t>
-  </si>
-  <si>
-    <t>RICHER</t>
-  </si>
-  <si>
-    <t>B.HORNES</t>
-  </si>
-  <si>
-    <t>B.SELAYARAN</t>
-  </si>
-  <si>
-    <t>GUILHERME</t>
-  </si>
-  <si>
-    <t>06H_OP1</t>
   </si>
   <si>
     <t>RODRIGO</t>
@@ -246,7 +246,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -262,6 +262,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFE699"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -293,7 +299,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -306,6 +312,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -687,10 +696,10 @@
         <v>34</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>50</v>
@@ -737,37 +746,37 @@
         <v>35</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D5" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F5" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="E5" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>38</v>
-      </c>
       <c r="G5" s="4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L5" s="4" t="s">
         <v>37</v>
       </c>
       <c r="M5" s="4">
+        <v>8</v>
+      </c>
+      <c r="N5" s="4">
         <v>6</v>
       </c>
-      <c r="N5" s="4">
-        <v>4</v>
-      </c>
       <c r="O5" s="4">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="P5" s="4">
         <v>4</v>
@@ -787,25 +796,25 @@
         <v>36</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D6" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F6" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="E6" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>38</v>
-      </c>
       <c r="G6" s="4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="L6" s="4" t="s">
         <v>49</v>
@@ -814,19 +823,19 @@
         <v>0</v>
       </c>
       <c r="N6" s="4">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="O6" s="4">
         <v>3</v>
       </c>
       <c r="P6" s="4">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="Q6" s="4">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="R6" s="5">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:18">
@@ -834,49 +843,49 @@
         <v>5</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="H7" s="4" t="s">
         <v>49</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="M7" s="4">
+        <v>10</v>
+      </c>
+      <c r="N7" s="4">
         <v>5</v>
       </c>
-      <c r="N7" s="4">
+      <c r="O7" s="4">
         <v>3</v>
       </c>
-      <c r="O7" s="4">
-        <v>7</v>
-      </c>
       <c r="P7" s="4">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="Q7" s="4">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="R7" s="5">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:18">
@@ -884,31 +893,31 @@
         <v>6</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="M8" s="4">
         <v>5</v>
@@ -917,16 +926,16 @@
         <v>5</v>
       </c>
       <c r="O8" s="4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P8" s="4">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="Q8" s="4">
-        <v>20</v>
-      </c>
-      <c r="R8" s="5">
-        <v>11</v>
+        <v>22</v>
+      </c>
+      <c r="R8" s="4">
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:18">
@@ -934,13 +943,13 @@
         <v>7</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>44</v>
@@ -949,34 +958,34 @@
         <v>49</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="H9" s="4" t="s">
         <v>38</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="L9" s="4" t="s">
         <v>35</v>
       </c>
       <c r="M9" s="4">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="N9" s="4">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="O9" s="4">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="P9" s="4">
         <v>2</v>
       </c>
       <c r="Q9" s="4">
-        <v>18</v>
-      </c>
-      <c r="R9" s="5">
-        <v>13</v>
+        <v>22</v>
+      </c>
+      <c r="R9" s="4">
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:18">
@@ -984,49 +993,49 @@
         <v>8</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>43</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="I10" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="L10" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="L10" s="4" t="s">
-        <v>40</v>
-      </c>
       <c r="M10" s="4">
+        <v>0</v>
+      </c>
+      <c r="N10" s="4">
+        <v>8</v>
+      </c>
+      <c r="O10" s="4">
         <v>4</v>
       </c>
-      <c r="N10" s="4">
-        <v>5</v>
-      </c>
-      <c r="O10" s="4">
-        <v>6</v>
-      </c>
       <c r="P10" s="4">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="Q10" s="4">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="R10" s="5">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:18">
@@ -1034,49 +1043,49 @@
         <v>9</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D11" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="H11" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="E11" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>36</v>
-      </c>
       <c r="I11" s="4" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="L11" s="4" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="M11" s="4">
+        <v>0</v>
+      </c>
+      <c r="N11" s="4">
+        <v>1</v>
+      </c>
+      <c r="O11" s="4">
         <v>7</v>
       </c>
-      <c r="N11" s="4">
-        <v>3</v>
-      </c>
-      <c r="O11" s="4">
-        <v>1</v>
-      </c>
       <c r="P11" s="4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="Q11" s="4">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="R11" s="5">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:18">
@@ -1084,49 +1093,49 @@
         <v>10</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="L12" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="M12" s="4">
+        <v>4</v>
+      </c>
+      <c r="N12" s="4">
+        <v>3</v>
+      </c>
+      <c r="O12" s="4">
         <v>9</v>
       </c>
-      <c r="N12" s="4">
-        <v>2</v>
-      </c>
-      <c r="O12" s="4">
-        <v>8</v>
-      </c>
       <c r="P12" s="4">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="Q12" s="4">
-        <v>21</v>
-      </c>
-      <c r="R12" s="5">
-        <v>10</v>
+        <v>22</v>
+      </c>
+      <c r="R12" s="4">
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:18">
@@ -1134,49 +1143,49 @@
         <v>11</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="L13" s="4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="M13" s="4">
+        <v>4</v>
+      </c>
+      <c r="N13" s="4">
+        <v>4</v>
+      </c>
+      <c r="O13" s="4">
         <v>7</v>
-      </c>
-      <c r="N13" s="4">
-        <v>7</v>
-      </c>
-      <c r="O13" s="4">
-        <v>2</v>
       </c>
       <c r="P13" s="4">
         <v>5</v>
       </c>
       <c r="Q13" s="4">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="R13" s="5">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:18">
@@ -1184,40 +1193,40 @@
         <v>12</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>35</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F14" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="H14" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="G14" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="H14" s="4" t="s">
-        <v>40</v>
-      </c>
       <c r="I14" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="L14" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="L14" s="4" t="s">
-        <v>46</v>
-      </c>
       <c r="M14" s="4">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="N14" s="4">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="O14" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P14" s="4">
         <v>0</v>
@@ -1234,43 +1243,43 @@
         <v>13</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>43</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="H15" s="4" t="s">
         <v>49</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L15" s="4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="M15" s="4">
+        <v>3</v>
+      </c>
+      <c r="N15" s="4">
+        <v>6</v>
+      </c>
+      <c r="O15" s="4">
         <v>2</v>
       </c>
-      <c r="N15" s="4">
-        <v>8</v>
-      </c>
-      <c r="O15" s="4">
-        <v>6</v>
-      </c>
       <c r="P15" s="4">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="Q15" s="4">
         <v>22</v>
@@ -1284,49 +1293,49 @@
         <v>14</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="L16" s="4" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="M16" s="4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="N16" s="4">
+        <v>9</v>
+      </c>
+      <c r="O16" s="4">
+        <v>3</v>
+      </c>
+      <c r="P16" s="4">
         <v>6</v>
       </c>
-      <c r="O16" s="4">
+      <c r="Q16" s="4">
+        <v>22</v>
+      </c>
+      <c r="R16" s="4">
         <v>9</v>
-      </c>
-      <c r="P16" s="4">
-        <v>5</v>
-      </c>
-      <c r="Q16" s="4">
-        <v>21</v>
-      </c>
-      <c r="R16" s="5">
-        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:18">
@@ -1334,49 +1343,49 @@
         <v>15</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="H17" s="4" t="s">
         <v>49</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="L17" s="4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="M17" s="4">
+        <v>6</v>
+      </c>
+      <c r="N17" s="4">
+        <v>5</v>
+      </c>
+      <c r="O17" s="4">
+        <v>7</v>
+      </c>
+      <c r="P17" s="4">
         <v>3</v>
       </c>
-      <c r="N17" s="4">
-        <v>2</v>
-      </c>
-      <c r="O17" s="4">
-        <v>4</v>
-      </c>
-      <c r="P17" s="4">
-        <v>13</v>
-      </c>
       <c r="Q17" s="4">
-        <v>22</v>
-      </c>
-      <c r="R17" s="4">
-        <v>9</v>
+        <v>21</v>
+      </c>
+      <c r="R17" s="5">
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:18">
@@ -1384,28 +1393,28 @@
         <v>16</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19" spans="1:18">
@@ -1413,28 +1422,28 @@
         <v>17</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="I19" s="4" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:18">
@@ -1442,28 +1451,28 @@
         <v>18</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:18">
@@ -1474,25 +1483,25 @@
         <v>36</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I21" s="4" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="22" spans="1:18">
@@ -1500,28 +1509,28 @@
         <v>20</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="I22" s="4" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="23" spans="1:18">
@@ -1529,28 +1538,28 @@
         <v>21</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C23" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="H23" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="D23" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="F23" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="G23" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="H23" s="4" t="s">
-        <v>40</v>
-      </c>
       <c r="I23" s="4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="24" spans="1:18">
@@ -1558,25 +1567,25 @@
         <v>22</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="I24" s="4" t="s">
         <v>44</v>
@@ -1587,28 +1596,28 @@
         <v>23</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E25" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="H25" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="F25" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="G25" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="H25" s="4" t="s">
-        <v>36</v>
-      </c>
       <c r="I25" s="4" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="26" spans="1:18">
@@ -1616,28 +1625,28 @@
         <v>24</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="I26" s="4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="27" spans="1:18">
@@ -1645,28 +1654,28 @@
         <v>25</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E27" s="4" t="s">
         <v>43</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="I27" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="28" spans="1:18">
@@ -1674,28 +1683,28 @@
         <v>26</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="E28" s="4" t="s">
         <v>44</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="I28" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="29" spans="1:18">
@@ -1706,25 +1715,25 @@
         <v>37</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I29" s="4" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
     </row>
     <row r="30" spans="1:18">
@@ -1735,25 +1744,25 @@
         <v>35</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D30" s="4" t="s">
         <v>36</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="F30" s="4" t="s">
         <v>38</v>
       </c>
       <c r="G30" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="H30" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="H30" s="4" t="s">
-        <v>37</v>
-      </c>
       <c r="I30" s="4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="31" spans="1:18">
@@ -1761,22 +1770,22 @@
         <v>29</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E31" s="4" t="s">
         <v>44</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H31" s="4" t="s">
         <v>38</v>
@@ -1790,25 +1799,25 @@
         <v>30</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="H32" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I32" s="4" t="s">
         <v>43</v>
@@ -1819,28 +1828,28 @@
         <v>31</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G33" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="H33" s="4" t="s">
-        <v>38</v>
+      <c r="H33" s="6" t="s">
+        <v>49</v>
       </c>
       <c r="I33" s="4" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
     </row>
     <row r="34" spans="1:9">
@@ -1848,25 +1857,25 @@
         <v>32</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="H34" s="4" t="s">
-        <v>40</v>
+        <v>42</v>
+      </c>
+      <c r="H34" s="6" t="s">
+        <v>49</v>
       </c>
       <c r="I34" s="4" t="s">
         <v>43</v>
@@ -1877,28 +1886,28 @@
         <v>33</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I35" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -1927,7 +1936,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="4" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B2" s="4">
         <v>132</v>
@@ -1935,7 +1944,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="4" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="B3" s="4">
         <v>132</v>
@@ -1943,31 +1952,31 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="4" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B4" s="4">
-        <v>126</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B5" s="4">
-        <v>126</v>
+        <v>132</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B6" s="4">
-        <v>126</v>
+        <v>132</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B7" s="4">
         <v>126</v>
@@ -1975,15 +1984,15 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="4" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="B8" s="4">
-        <v>126</v>
+        <v>120</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B9" s="4">
         <v>120</v>
@@ -1991,7 +2000,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="4" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="B10" s="4">
         <v>120</v>
@@ -1999,34 +2008,34 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="4" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="B11" s="4">
-        <v>108</v>
+        <v>102</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B12" s="4">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="4" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="B13" s="4">
-        <v>84</v>
+        <v>72</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B14" s="4">
-        <v>60</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add validação de periodo entre as folgas ser no mewsmo turno
</commit_message>
<xml_diff>
--- a/ESCALA_TORRE_V5.xlsx
+++ b/ESCALA_TORRE_V5.xlsx
@@ -122,12 +122,12 @@
     <t>00H_OP1</t>
   </si>
   <si>
+    <t>EDUARDO</t>
+  </si>
+  <si>
     <t>BRANCÃO</t>
   </si>
   <si>
-    <t>EDUARDO</t>
-  </si>
-  <si>
     <t>ALLAN</t>
   </si>
   <si>
@@ -137,34 +137,34 @@
     <t>00H_OP2</t>
   </si>
   <si>
+    <t>B.HORNES</t>
+  </si>
+  <si>
+    <t>RICHER</t>
+  </si>
+  <si>
+    <t>GUILHERME</t>
+  </si>
+  <si>
     <t>THAIS</t>
   </si>
   <si>
-    <t>RICHER</t>
-  </si>
-  <si>
-    <t>B.HORNES</t>
-  </si>
-  <si>
-    <t>GUILHERME</t>
+    <t>B.SELAYARAN</t>
   </si>
   <si>
     <t>FELIPE</t>
   </si>
   <si>
-    <t>B.SELAYARAN</t>
-  </si>
-  <si>
     <t>06H_OP1</t>
   </si>
   <si>
+    <t>RODRIGO</t>
+  </si>
+  <si>
     <t>CLEITON</t>
   </si>
   <si>
     <t>TONINHO</t>
-  </si>
-  <si>
-    <t>RODRIGO</t>
   </si>
   <si>
     <t>06H_OP2</t>
@@ -749,43 +749,43 @@
         <v>40</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L5" s="4" t="s">
         <v>37</v>
       </c>
       <c r="M5" s="4">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="N5" s="4">
         <v>6</v>
       </c>
       <c r="O5" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P5" s="4">
         <v>4</v>
       </c>
       <c r="Q5" s="4">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="R5" s="5">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:18">
@@ -799,43 +799,43 @@
         <v>41</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="M6" s="4">
         <v>0</v>
       </c>
       <c r="N6" s="4">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="O6" s="4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="P6" s="4">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="Q6" s="4">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="R6" s="5">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:18">
@@ -843,49 +843,49 @@
         <v>5</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>42</v>
       </c>
       <c r="D7" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="H7" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="E7" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>49</v>
-      </c>
       <c r="I7" s="4" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="M7" s="4">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="N7" s="4">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="O7" s="4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="P7" s="4">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="Q7" s="4">
-        <v>20</v>
-      </c>
-      <c r="R7" s="5">
-        <v>11</v>
+        <v>22</v>
+      </c>
+      <c r="R7" s="4">
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:18">
@@ -896,34 +896,34 @@
         <v>36</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>47</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>35</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="L8" s="4" t="s">
         <v>38</v>
       </c>
       <c r="M8" s="4">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="N8" s="4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="O8" s="4">
         <v>5</v>
@@ -943,49 +943,49 @@
         <v>7</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="D9" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F9" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="G9" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="I9" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="F9" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="I9" s="4" t="s">
-        <v>41</v>
-      </c>
       <c r="L9" s="4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="M9" s="4">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="N9" s="4">
+        <v>3</v>
+      </c>
+      <c r="O9" s="4">
         <v>5</v>
       </c>
-      <c r="O9" s="4">
-        <v>7</v>
-      </c>
       <c r="P9" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Q9" s="4">
-        <v>22</v>
-      </c>
-      <c r="R9" s="4">
-        <v>9</v>
+        <v>21</v>
+      </c>
+      <c r="R9" s="5">
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:18">
@@ -993,49 +993,49 @@
         <v>8</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>38</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="I10" s="4" t="s">
         <v>40</v>
       </c>
       <c r="L10" s="4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="M10" s="4">
         <v>0</v>
       </c>
       <c r="N10" s="4">
+        <v>5</v>
+      </c>
+      <c r="O10" s="4">
         <v>8</v>
       </c>
-      <c r="O10" s="4">
-        <v>4</v>
-      </c>
       <c r="P10" s="4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="Q10" s="4">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="R10" s="5">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:18">
@@ -1043,31 +1043,31 @@
         <v>9</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H11" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="L11" s="4" t="s">
         <v>49</v>
-      </c>
-      <c r="I11" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="L11" s="4" t="s">
-        <v>48</v>
       </c>
       <c r="M11" s="4">
         <v>0</v>
@@ -1076,16 +1076,16 @@
         <v>1</v>
       </c>
       <c r="O11" s="4">
+        <v>5</v>
+      </c>
+      <c r="P11" s="4">
         <v>7</v>
       </c>
-      <c r="P11" s="4">
-        <v>4</v>
-      </c>
       <c r="Q11" s="4">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="R11" s="5">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:18">
@@ -1096,40 +1096,40 @@
         <v>36</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="L12" s="4" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="M12" s="4">
+        <v>5</v>
+      </c>
+      <c r="N12" s="4">
         <v>4</v>
       </c>
-      <c r="N12" s="4">
-        <v>3</v>
-      </c>
       <c r="O12" s="4">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="P12" s="4">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="Q12" s="4">
         <v>22</v>
@@ -1143,49 +1143,49 @@
         <v>11</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D13" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F13" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="E13" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>35</v>
-      </c>
       <c r="G13" s="4" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="L13" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="M13" s="4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="N13" s="4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="O13" s="4">
+        <v>8</v>
+      </c>
+      <c r="P13" s="4">
         <v>7</v>
       </c>
-      <c r="P13" s="4">
-        <v>5</v>
-      </c>
       <c r="Q13" s="4">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="R13" s="5">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:18">
@@ -1193,43 +1193,43 @@
         <v>12</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G14" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="L14" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="H14" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="I14" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="L14" s="4" t="s">
-        <v>45</v>
-      </c>
       <c r="M14" s="4">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="N14" s="4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="O14" s="4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P14" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q14" s="4">
         <v>17</v>
@@ -1243,49 +1243,49 @@
         <v>13</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>47</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L15" s="4" t="s">
         <v>41</v>
       </c>
       <c r="M15" s="4">
+        <v>5</v>
+      </c>
+      <c r="N15" s="4">
+        <v>8</v>
+      </c>
+      <c r="O15" s="4">
+        <v>4</v>
+      </c>
+      <c r="P15" s="4">
         <v>3</v>
       </c>
-      <c r="N15" s="4">
-        <v>6</v>
-      </c>
-      <c r="O15" s="4">
-        <v>2</v>
-      </c>
-      <c r="P15" s="4">
+      <c r="Q15" s="4">
+        <v>20</v>
+      </c>
+      <c r="R15" s="5">
         <v>11</v>
-      </c>
-      <c r="Q15" s="4">
-        <v>22</v>
-      </c>
-      <c r="R15" s="4">
-        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:18">
@@ -1293,43 +1293,43 @@
         <v>14</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="L16" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="M16" s="4">
         <v>4</v>
       </c>
       <c r="N16" s="4">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="O16" s="4">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="P16" s="4">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="Q16" s="4">
         <v>22</v>
@@ -1349,43 +1349,43 @@
         <v>44</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>43</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="G17" s="4" t="s">
         <v>45</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L17" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="M17" s="4">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="N17" s="4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="O17" s="4">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="P17" s="4">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="Q17" s="4">
-        <v>21</v>
-      </c>
-      <c r="R17" s="5">
-        <v>10</v>
+        <v>22</v>
+      </c>
+      <c r="R17" s="4">
+        <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:18">
@@ -1393,7 +1393,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>42</v>
@@ -1402,19 +1402,19 @@
         <v>37</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F18" s="4" t="s">
         <v>38</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:18">
@@ -1422,28 +1422,28 @@
         <v>17</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D19" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="H19" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="E19" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="H19" s="4" t="s">
-        <v>48</v>
-      </c>
       <c r="I19" s="4" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20" spans="1:18">
@@ -1451,28 +1451,28 @@
         <v>18</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:18">
@@ -1480,28 +1480,28 @@
         <v>19</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="F21" s="4" t="s">
         <v>48</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="I21" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:18">
@@ -1512,25 +1512,25 @@
         <v>37</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="G22" s="4" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="I22" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="23" spans="1:18">
@@ -1538,25 +1538,25 @@
         <v>21</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C23" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="G23" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="D23" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="F23" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="G23" s="4" t="s">
-        <v>41</v>
-      </c>
       <c r="H23" s="4" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="I23" s="4" t="s">
         <v>42</v>
@@ -1567,28 +1567,28 @@
         <v>22</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>40</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="I24" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="25" spans="1:18">
@@ -1596,28 +1596,28 @@
         <v>23</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="G25" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="I25" s="4" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="26" spans="1:18">
@@ -1628,25 +1628,25 @@
         <v>38</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="I26" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="27" spans="1:18">
@@ -1654,28 +1654,28 @@
         <v>25</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G27" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="H27" s="4" t="s">
-        <v>37</v>
+        <v>43</v>
+      </c>
+      <c r="H27" s="6" t="s">
+        <v>47</v>
       </c>
       <c r="I27" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="28" spans="1:18">
@@ -1683,25 +1683,25 @@
         <v>26</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="I28" s="4" t="s">
         <v>41</v>
@@ -1712,25 +1712,25 @@
         <v>27</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F29" s="4" t="s">
         <v>48</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="I29" s="4" t="s">
         <v>40</v>
@@ -1741,25 +1741,25 @@
         <v>28</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H30" s="4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="I30" s="4" t="s">
         <v>42</v>
@@ -1770,22 +1770,22 @@
         <v>29</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E31" s="4" t="s">
         <v>44</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H31" s="4" t="s">
         <v>38</v>
@@ -1799,28 +1799,28 @@
         <v>30</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="F32" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="H32" s="4" t="s">
         <v>36</v>
       </c>
       <c r="I32" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="33" spans="1:9">
@@ -1828,28 +1828,28 @@
         <v>31</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D33" s="4" t="s">
         <v>37</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="H33" s="6" t="s">
-        <v>49</v>
+        <v>42</v>
+      </c>
+      <c r="H33" s="4" t="s">
+        <v>35</v>
       </c>
       <c r="I33" s="4" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
     </row>
     <row r="34" spans="1:9">
@@ -1857,28 +1857,28 @@
         <v>32</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C34" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E34" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="D34" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="E34" s="4" t="s">
-        <v>45</v>
-      </c>
       <c r="F34" s="4" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H34" s="6" t="s">
         <v>49</v>
       </c>
       <c r="I34" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="35" spans="1:9">
@@ -1886,28 +1886,28 @@
         <v>33</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="G35" s="4" t="s">
         <v>40</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="I35" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1936,7 +1936,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B2" s="4">
         <v>132</v>
@@ -1944,7 +1944,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="4" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B3" s="4">
         <v>132</v>
@@ -1952,7 +1952,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="4" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B4" s="4">
         <v>132</v>
@@ -1960,7 +1960,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B5" s="4">
         <v>132</v>
@@ -1968,7 +1968,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B6" s="4">
         <v>132</v>
@@ -1976,7 +1976,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="4" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B7" s="4">
         <v>126</v>
@@ -1984,23 +1984,23 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B8" s="4">
-        <v>120</v>
+        <v>126</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="4" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="B9" s="4">
-        <v>120</v>
+        <v>126</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B10" s="4">
         <v>120</v>
@@ -2008,7 +2008,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B11" s="4">
         <v>102</v>
@@ -2016,10 +2016,10 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B12" s="4">
-        <v>96</v>
+        <v>84</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -2027,15 +2027,15 @@
         <v>49</v>
       </c>
       <c r="B13" s="4">
-        <v>72</v>
+        <v>78</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B14" s="4">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>